<commit_message>
Updated table of responsibilities
</commit_message>
<xml_diff>
--- a/Dorm Community Handbook/images/03 Organization/kitchen-responsibilities.xlsx
+++ b/Dorm Community Handbook/images/03 Organization/kitchen-responsibilities.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robin/git-robin/community-handbook/Dorm Community Handbook/images/05 Responsibilities/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lucascaputogoncalves/Desktop/Fichtenweg 17U/community-handbook/Dorm Community Handbook/images/03 Organization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D9F16B4A-3DED-7C4F-A71C-D5476C415578}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EA276C6-0F97-4149-89CB-A88E9F33F800}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11880" yWindow="6000" windowWidth="27840" windowHeight="16740" xr2:uid="{DE47AEF3-7EE9-414A-A4C6-77EF2BA50DD5}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{DE47AEF3-7EE9-414A-A4C6-77EF2BA50DD5}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
   <si>
     <t>Responsibility</t>
   </si>
@@ -59,25 +59,64 @@
     <t>Oven</t>
   </si>
   <si>
-    <t>Dishes</t>
-  </si>
-  <si>
-    <t>Table &amp; Cooking surfaces</t>
-  </si>
-  <si>
     <t>Toaster &amp; Kettle</t>
   </si>
   <si>
     <t>Microwave</t>
   </si>
   <si>
-    <t>Floor &amp; Shelves</t>
-  </si>
-  <si>
     <t>Robin Epple</t>
   </si>
   <si>
     <t>U 13</t>
+  </si>
+  <si>
+    <t>Silvy Kurzendorfer</t>
+  </si>
+  <si>
+    <t>U 17</t>
+  </si>
+  <si>
+    <t>U 09</t>
+  </si>
+  <si>
+    <t>Table &amp; Chairs</t>
+  </si>
+  <si>
+    <t>Cooking Surfaces</t>
+  </si>
+  <si>
+    <t>Garbage &amp; Area around</t>
+  </si>
+  <si>
+    <t>Dishes &amp; Washing Utilities</t>
+  </si>
+  <si>
+    <t>Floor &amp; Window Sill</t>
+  </si>
+  <si>
+    <t>Shelves</t>
+  </si>
+  <si>
+    <t>Michael Stengel</t>
+  </si>
+  <si>
+    <t>U 08</t>
+  </si>
+  <si>
+    <t>U 06</t>
+  </si>
+  <si>
+    <t>Danny Löser?</t>
+  </si>
+  <si>
+    <t>Pans, Pots, etc.</t>
+  </si>
+  <si>
+    <t>Luke Caputo G.</t>
+  </si>
+  <si>
+    <t>Sink &amp; Wall behind</t>
   </si>
 </sst>
 </file>
@@ -129,7 +168,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -145,7 +184,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -461,10 +500,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66A41B80-3ED8-6E46-9A7A-5BA065A4B20A}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" zoomScale="179" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -490,59 +529,115 @@
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>7</v>
+        <v>17</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>10</v>
+        <v>4</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>9</v>
+        <v>15</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Table and Stellan intro
</commit_message>
<xml_diff>
--- a/Dorm Community Handbook/images/03 Organization/kitchen-responsibilities.xlsx
+++ b/Dorm Community Handbook/images/03 Organization/kitchen-responsibilities.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lucascaputogoncalves/Desktop/Fichtenweg 17U/community-handbook/Dorm Community Handbook/images/03 Organization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CEC979A-655B-A64D-B40D-178CD7776E84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4363A8A3-5724-B549-B3B0-FFBE877DE138}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{DE47AEF3-7EE9-414A-A4C6-77EF2BA50DD5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
   <si>
     <t>Responsibility</t>
   </si>
@@ -117,6 +117,12 @@
   </si>
   <si>
     <t>Toaster, Kettle &amp; Sandwich Maker</t>
+  </si>
+  <si>
+    <t>Luke C. and Bogdan T.</t>
+  </si>
+  <si>
+    <t>U 09 &amp; U 16</t>
   </si>
 </sst>
 </file>
@@ -503,7 +509,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="179" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -636,6 +642,12 @@
       <c r="A14" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="B14" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">

</xml_diff>